<commit_message>
Buglist updated with latest status
</commit_message>
<xml_diff>
--- a/defects/BugList-V1_0-2.xlsx
+++ b/defects/BugList-V1_0-2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="150">
   <si>
     <t>Bug Number</t>
   </si>
@@ -589,6 +589,9 @@
   </si>
   <si>
     <t>Need clarification</t>
+  </si>
+  <si>
+    <t>A flag "gestationRecord" is set as true when gestation window is opened</t>
   </si>
 </sst>
 </file>
@@ -764,12 +767,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -791,6 +788,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,7 +1066,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1229,7 +1232,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1395,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,35 +1573,35 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="30">
         <v>9</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="32" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="16"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="23"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="29"/>
       <c r="J9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="16"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="23"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="29"/>
       <c r="J10" t="s">
         <v>115</v>
       </c>
@@ -1958,30 +1961,30 @@
       <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
+      <c r="A35" s="30">
         <v>34</v>
       </c>
-      <c r="B35" s="21"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="21"/>
+      <c r="D35" s="31"/>
       <c r="E35" s="18"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="23"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="29"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="21"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="18"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="23"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="29"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
@@ -1998,30 +2001,30 @@
       <c r="H37" s="19"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
+      <c r="A38" s="30">
         <v>36</v>
       </c>
-      <c r="B38" s="21"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="21"/>
+      <c r="D38" s="31"/>
       <c r="E38" s="18"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="23"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="29"/>
     </row>
     <row r="39" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="21"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="21"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="23"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="29"/>
     </row>
     <row r="40" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
@@ -2437,7 +2440,7 @@
       <c r="C64" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D64" s="24"/>
+      <c r="D64" s="20"/>
       <c r="E64" s="18" t="s">
         <v>102</v>
       </c>
@@ -2454,7 +2457,7 @@
         <v>57</v>
       </c>
       <c r="B65" s="18"/>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="21" t="s">
         <v>117</v>
       </c>
       <c r="D65" s="18"/>
@@ -2470,29 +2473,29 @@
       </c>
     </row>
     <row r="66" spans="1:8" s="14" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="26">
+      <c r="A66" s="22">
         <v>58</v>
       </c>
-      <c r="B66" s="26"/>
-      <c r="C66" s="27" t="s">
+      <c r="B66" s="22"/>
+      <c r="C66" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="D66" s="26"/>
+      <c r="D66" s="22"/>
       <c r="E66" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F66" s="26" t="s">
+      <c r="F66" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="G66" s="26"/>
-      <c r="H66" s="28"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="24"/>
     </row>
     <row r="67" spans="1:8" ht="39" x14ac:dyDescent="0.25">
       <c r="A67" s="18">
         <v>59</v>
       </c>
       <c r="B67" s="18"/>
-      <c r="C67" s="25" t="s">
+      <c r="C67" s="21" t="s">
         <v>122</v>
       </c>
       <c r="D67" s="18"/>
@@ -2500,7 +2503,7 @@
         <v>102</v>
       </c>
       <c r="F67" s="18" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="G67" s="18"/>
       <c r="H67" s="19"/>
@@ -2510,7 +2513,7 @@
         <v>60</v>
       </c>
       <c r="B68" s="18"/>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="21" t="s">
         <v>123</v>
       </c>
       <c r="D68" s="18"/>
@@ -2518,9 +2521,11 @@
         <v>102</v>
       </c>
       <c r="F68" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="G68" s="18"/>
+        <v>136</v>
+      </c>
+      <c r="G68" s="18" t="s">
+        <v>149</v>
+      </c>
       <c r="H68" s="19"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2528,7 +2533,7 @@
         <v>61</v>
       </c>
       <c r="B69" s="18"/>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="21" t="s">
         <v>124</v>
       </c>
       <c r="D69" s="18"/>
@@ -2536,7 +2541,7 @@
         <v>102</v>
       </c>
       <c r="F69" s="18" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="G69" s="18"/>
       <c r="H69" s="19"/>
@@ -2546,7 +2551,7 @@
         <v>62</v>
       </c>
       <c r="B70" s="18"/>
-      <c r="C70" s="25" t="s">
+      <c r="C70" s="21" t="s">
         <v>125</v>
       </c>
       <c r="D70" s="18"/>
@@ -2564,7 +2569,7 @@
         <v>63</v>
       </c>
       <c r="B71" s="18"/>
-      <c r="C71" s="25" t="s">
+      <c r="C71" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D71" s="18"/>
@@ -2584,7 +2589,7 @@
         <v>64</v>
       </c>
       <c r="B72" s="18"/>
-      <c r="C72" s="25" t="s">
+      <c r="C72" s="21" t="s">
         <v>127</v>
       </c>
       <c r="D72" s="18"/>
@@ -2604,7 +2609,7 @@
         <v>65</v>
       </c>
       <c r="B73" s="18"/>
-      <c r="C73" s="25" t="s">
+      <c r="C73" s="21" t="s">
         <v>118</v>
       </c>
       <c r="D73" s="18"/>
@@ -2612,7 +2617,7 @@
         <v>102</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="G73" s="18"/>
       <c r="H73" s="19"/>
@@ -2622,7 +2627,7 @@
         <v>66</v>
       </c>
       <c r="B74" s="18"/>
-      <c r="C74" s="25" t="s">
+      <c r="C74" s="21" t="s">
         <v>128</v>
       </c>
       <c r="D74" s="18"/>
@@ -2640,7 +2645,7 @@
         <v>67</v>
       </c>
       <c r="B75" s="18"/>
-      <c r="C75" s="25" t="s">
+      <c r="C75" s="21" t="s">
         <v>129</v>
       </c>
       <c r="D75" s="18"/>
@@ -2658,7 +2663,7 @@
         <v>67</v>
       </c>
       <c r="B76" s="18"/>
-      <c r="C76" s="25" t="s">
+      <c r="C76" s="21" t="s">
         <v>119</v>
       </c>
       <c r="D76" s="18"/>
@@ -2676,7 +2681,7 @@
         <v>68</v>
       </c>
       <c r="B77" s="18"/>
-      <c r="C77" s="25" t="s">
+      <c r="C77" s="21" t="s">
         <v>120</v>
       </c>
       <c r="D77" s="18"/>
@@ -2694,7 +2699,7 @@
         <v>69</v>
       </c>
       <c r="B78" s="18"/>
-      <c r="C78" s="25" t="s">
+      <c r="C78" s="21" t="s">
         <v>121</v>
       </c>
       <c r="D78" s="18"/>
@@ -2708,310 +2713,316 @@
       <c r="H78" s="19"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="29">
+      <c r="A79" s="25">
         <v>70</v>
       </c>
-      <c r="B79" s="29"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
-      <c r="G79" s="29"/>
-      <c r="H79" s="31"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="25"/>
+      <c r="H79" s="27"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="29">
+      <c r="A80" s="25">
         <v>71</v>
       </c>
-      <c r="B80" s="29"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
-      <c r="G80" s="29"/>
-      <c r="H80" s="31"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="27"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="29">
+      <c r="A81" s="25">
         <v>72</v>
       </c>
-      <c r="B81" s="29"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="29"/>
-      <c r="E81" s="29"/>
-      <c r="F81" s="29"/>
-      <c r="G81" s="29"/>
-      <c r="H81" s="31"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="25"/>
+      <c r="H81" s="27"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="29">
+      <c r="A82" s="25">
         <v>73</v>
       </c>
-      <c r="B82" s="29"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="29"/>
-      <c r="E82" s="29"/>
-      <c r="F82" s="29"/>
-      <c r="G82" s="29"/>
-      <c r="H82" s="31"/>
+      <c r="B82" s="25"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="25"/>
+      <c r="H82" s="27"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="29">
+      <c r="A83" s="25">
         <v>74</v>
       </c>
-      <c r="B83" s="29"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
-      <c r="G83" s="29"/>
-      <c r="H83" s="31"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="25"/>
+      <c r="H83" s="27"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="29">
+      <c r="A84" s="25">
         <v>75</v>
       </c>
-      <c r="B84" s="29"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
-      <c r="G84" s="29"/>
-      <c r="H84" s="31"/>
+      <c r="B84" s="25"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="25"/>
+      <c r="G84" s="25"/>
+      <c r="H84" s="27"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="29">
+      <c r="A85" s="25">
         <v>76</v>
       </c>
-      <c r="B85" s="29"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
-      <c r="G85" s="29"/>
-      <c r="H85" s="31"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="25"/>
+      <c r="H85" s="27"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="29">
+      <c r="A86" s="25">
         <v>77</v>
       </c>
-      <c r="B86" s="29"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="29"/>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
-      <c r="G86" s="29"/>
-      <c r="H86" s="31"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="25"/>
+      <c r="H86" s="27"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="29">
+      <c r="A87" s="25">
         <v>78</v>
       </c>
-      <c r="B87" s="29"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="29"/>
-      <c r="H87" s="31"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="27"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="29">
+      <c r="A88" s="25">
         <v>79</v>
       </c>
-      <c r="B88" s="29"/>
-      <c r="C88" s="32"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="29"/>
-      <c r="G88" s="29"/>
-      <c r="H88" s="31"/>
+      <c r="B88" s="25"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="25"/>
+      <c r="H88" s="27"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="29">
+      <c r="A89" s="25">
         <v>80</v>
       </c>
-      <c r="B89" s="29"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="29"/>
-      <c r="E89" s="29"/>
-      <c r="F89" s="29"/>
-      <c r="G89" s="29"/>
-      <c r="H89" s="31"/>
+      <c r="B89" s="25"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="25"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="25"/>
+      <c r="G89" s="25"/>
+      <c r="H89" s="27"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="29">
+      <c r="A90" s="25">
         <v>81</v>
       </c>
-      <c r="B90" s="29"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="31"/>
+      <c r="B90" s="25"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="25"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="25"/>
+      <c r="H90" s="27"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="29">
+      <c r="A91" s="25">
         <v>82</v>
       </c>
-      <c r="B91" s="29"/>
-      <c r="C91" s="32"/>
-      <c r="D91" s="29"/>
-      <c r="E91" s="29"/>
-      <c r="F91" s="29"/>
-      <c r="G91" s="29"/>
-      <c r="H91" s="31"/>
+      <c r="B91" s="25"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="25"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="25"/>
+      <c r="G91" s="25"/>
+      <c r="H91" s="27"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="29">
+      <c r="A92" s="25">
         <v>83</v>
       </c>
-      <c r="B92" s="29"/>
-      <c r="C92" s="32"/>
-      <c r="D92" s="29"/>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
-      <c r="G92" s="29"/>
-      <c r="H92" s="31"/>
+      <c r="B92" s="25"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="25"/>
+      <c r="G92" s="25"/>
+      <c r="H92" s="27"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="29">
+      <c r="A93" s="25">
         <v>84</v>
       </c>
-      <c r="B93" s="29"/>
-      <c r="C93" s="32"/>
-      <c r="D93" s="29"/>
-      <c r="E93" s="29"/>
-      <c r="F93" s="29"/>
-      <c r="G93" s="29"/>
-      <c r="H93" s="31"/>
+      <c r="B93" s="25"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="25"/>
+      <c r="H93" s="27"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="29">
+      <c r="A94" s="25">
         <v>85</v>
       </c>
-      <c r="B94" s="29"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="31"/>
+      <c r="B94" s="25"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="25"/>
+      <c r="H94" s="27"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
-      <c r="B95" s="29"/>
-      <c r="C95" s="32"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="31"/>
+      <c r="A95" s="25"/>
+      <c r="B95" s="25"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="25"/>
+      <c r="G95" s="25"/>
+      <c r="H95" s="27"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="29"/>
-      <c r="B96" s="29"/>
-      <c r="C96" s="32"/>
-      <c r="D96" s="29"/>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
-      <c r="G96" s="29"/>
-      <c r="H96" s="31"/>
+      <c r="A96" s="25"/>
+      <c r="B96" s="25"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="25"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="25"/>
+      <c r="G96" s="25"/>
+      <c r="H96" s="27"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="29"/>
-      <c r="B97" s="29"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="29"/>
-      <c r="F97" s="29"/>
-      <c r="G97" s="29"/>
-      <c r="H97" s="31"/>
+      <c r="A97" s="25"/>
+      <c r="B97" s="25"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="25"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="25"/>
+      <c r="H97" s="27"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="29"/>
-      <c r="B98" s="29"/>
-      <c r="C98" s="32"/>
-      <c r="D98" s="29"/>
-      <c r="E98" s="29"/>
-      <c r="F98" s="29"/>
-      <c r="G98" s="29"/>
-      <c r="H98" s="31"/>
+      <c r="A98" s="25"/>
+      <c r="B98" s="25"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="25"/>
+      <c r="F98" s="25"/>
+      <c r="G98" s="25"/>
+      <c r="H98" s="27"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="29"/>
-      <c r="B99" s="29"/>
-      <c r="C99" s="32"/>
-      <c r="D99" s="29"/>
-      <c r="E99" s="29"/>
-      <c r="F99" s="29"/>
-      <c r="G99" s="29"/>
-      <c r="H99" s="31"/>
+      <c r="A99" s="25"/>
+      <c r="B99" s="25"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="25"/>
+      <c r="E99" s="25"/>
+      <c r="F99" s="25"/>
+      <c r="G99" s="25"/>
+      <c r="H99" s="27"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
-      <c r="B100" s="29"/>
-      <c r="C100" s="31"/>
-      <c r="D100" s="29"/>
-      <c r="E100" s="29"/>
-      <c r="F100" s="29"/>
-      <c r="G100" s="29"/>
-      <c r="H100" s="31"/>
+      <c r="A100" s="25"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="25"/>
+      <c r="H100" s="27"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
-      <c r="B101" s="29"/>
-      <c r="C101" s="31"/>
-      <c r="D101" s="29"/>
-      <c r="E101" s="29"/>
-      <c r="F101" s="29"/>
-      <c r="G101" s="29"/>
-      <c r="H101" s="31"/>
+      <c r="A101" s="25"/>
+      <c r="B101" s="25"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="25"/>
+      <c r="H101" s="27"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
-      <c r="B102" s="29"/>
-      <c r="C102" s="31"/>
-      <c r="D102" s="29"/>
-      <c r="E102" s="29"/>
-      <c r="F102" s="29"/>
-      <c r="G102" s="29"/>
-      <c r="H102" s="31"/>
+      <c r="A102" s="25"/>
+      <c r="B102" s="25"/>
+      <c r="C102" s="27"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="25"/>
+      <c r="H102" s="27"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="29"/>
-      <c r="B103" s="29"/>
-      <c r="C103" s="31"/>
-      <c r="D103" s="29"/>
-      <c r="E103" s="29"/>
-      <c r="F103" s="29"/>
-      <c r="G103" s="29"/>
-      <c r="H103" s="31"/>
+      <c r="A103" s="25"/>
+      <c r="B103" s="25"/>
+      <c r="C103" s="27"/>
+      <c r="D103" s="25"/>
+      <c r="E103" s="25"/>
+      <c r="F103" s="25"/>
+      <c r="G103" s="25"/>
+      <c r="H103" s="27"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="29"/>
-      <c r="B104" s="29"/>
-      <c r="C104" s="31"/>
-      <c r="D104" s="29"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="29"/>
-      <c r="G104" s="29"/>
-      <c r="H104" s="31"/>
+      <c r="A104" s="25"/>
+      <c r="B104" s="25"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="25"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="25"/>
+      <c r="H104" s="27"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="29"/>
-      <c r="B105" s="29"/>
-      <c r="C105" s="31"/>
-      <c r="D105" s="29"/>
-      <c r="E105" s="29"/>
-      <c r="F105" s="29"/>
-      <c r="G105" s="29"/>
-      <c r="H105" s="31"/>
+      <c r="A105" s="25"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="27"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="25"/>
+      <c r="H105" s="27"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H45"/>
   <mergeCells count="18">
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
     <mergeCell ref="H38:H39"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="B35:B36"/>
@@ -3024,12 +3035,6 @@
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">

</xml_diff>